<commit_message>
Commit extend report group
</commit_message>
<xml_diff>
--- a/ZoodelAutomation_Maven/src/test/resources/testdata/testdata.xlsx
+++ b/ZoodelAutomation_Maven/src/test/resources/testdata/testdata.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jagruti\git\ZoodelAutomationWithMaven\ZoodelAutomation_Maven\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6CE493-8E49-4D1E-903D-DE600FE60F35}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B20CB72-3952-4045-8D7B-BF18C6ED08FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="4275" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Runmode</t>
   </si>
@@ -45,12 +46,6 @@
     <t>food</t>
   </si>
   <si>
-    <t>Health &amp; Beauty</t>
-  </si>
-  <si>
-    <t>healthcare_cosmetics_personal_care</t>
-  </si>
-  <si>
     <t>Metallurgy &amp; Chemicals</t>
   </si>
   <si>
@@ -58,6 +53,48 @@
   </si>
   <si>
     <t>CheckTitleOfHomePageLink</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Medical, Health &amp; Beauty</t>
+  </si>
+  <si>
+    <t>medical-health-beauty</t>
+  </si>
+  <si>
+    <t>CheckTitleOfHomePageLink2</t>
+  </si>
+  <si>
+    <t>Machinery &amp; Industry</t>
+  </si>
+  <si>
+    <t>Automotive</t>
+  </si>
+  <si>
+    <t>machinery_industrial_plant_hardware_parts_tools</t>
+  </si>
+  <si>
+    <t>automotive_vehicles_transportation_parts</t>
+  </si>
+  <si>
+    <t>CheckStaticLinks</t>
+  </si>
+  <si>
+    <t>About Us</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>Expected Data</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>News</t>
   </si>
 </sst>
 </file>
@@ -375,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,7 +427,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -416,19 +453,114 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B1B3FD7-DB43-4358-9958-E9514E7D89E9}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
       <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>